<commit_message>
Revisión escaleta guiones para Greco, ajustes en mapa 09-08
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/Escaleta CN_06_08_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion08/Escaleta CN_06_08_CO.xlsx
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CN_06_08_CO!$A$2:$U$53</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -3416,8 +3416,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5:P52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6305,26 +6305,26 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I12 I14:I52">

</xml_diff>